<commit_message>
introduced new functions and torsion check
</commit_message>
<xml_diff>
--- a/excel_files/trial.xlsx
+++ b/excel_files/trial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2545-Select BB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adnan.a\Documents\GitHub\Killa-Design-Structures-code\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA3E3FA2-3F02-4CDF-9510-B0D42ED7F056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F122C699-91B5-4EAF-9032-C5508738F6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BC36A015-FB8E-4349-A622-79A853CE7F2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{BC36A015-FB8E-4349-A622-79A853CE7F2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Conc Bm Flx Env - ACI 318-19" sheetId="1" r:id="rId1"/>
@@ -1028,7 +1028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B8FD85-DFD7-4813-8B04-9B49F453D919}">
   <dimension ref="A1:K171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -7010,8 +7010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2417925B-5F9F-4ABE-B90C-1F89736841CE}">
   <dimension ref="A1:N171"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7212,7 +7212,7 @@
         <v>22</v>
       </c>
       <c r="K5">
-        <v>145.54</v>
+        <v>4000</v>
       </c>
       <c r="L5">
         <v>1.6197999999999999</v>
@@ -7904,7 +7904,7 @@
         <v>22</v>
       </c>
       <c r="K21">
-        <v>1101.29</v>
+        <v>4000</v>
       </c>
       <c r="L21">
         <v>193.22739999999999</v>

</xml_diff>